<commit_message>
Increased the image size to 17000 x 17000, to better see the difference in the execution times of sequential and parallel code. Also  allocated the pixels dynamically to it, while altering the parallelized code to handle the race condition occuring when the histgoram array was filled. This was done by using reduction. Also dynamically allocated and freed up memory to ensure that stack di dnot get full due to the large image size.
</commit_message>
<xml_diff>
--- a/PDC_Assignment1.xlsx
+++ b/PDC_Assignment1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hadia\OpenMP_Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAE9E95-0F23-4831-8A16-2E8F4A6143B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4299652-02BD-4A67-9963-EBB17CF35E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7766C438-E750-47BE-8A94-A38E353BDC78}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7766C438-E750-47BE-8A94-A38E353BDC78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Sequential Code Execution Time (seconds)</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>Parallel (Dynamic)</t>
-  </si>
-  <si>
-    <t>No. Of Threads</t>
-  </si>
-  <si>
-    <t>Parallelized Code Execution Time</t>
   </si>
 </sst>
 </file>
@@ -261,34 +255,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.7099999999999997E-4</c:v>
+                  <c:v>2.0874109999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2299999999999999E-4</c:v>
+                  <c:v>2.582166</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.14E-4</c:v>
+                  <c:v>5.6043609999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8100000000000001E-4</c:v>
+                  <c:v>7.0913029999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.05E-4</c:v>
+                  <c:v>4.9783179999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.8199999999999999E-4</c:v>
+                  <c:v>1.6207819999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4399999999999999E-4</c:v>
+                  <c:v>4.5114200000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6000000000000001E-4</c:v>
+                  <c:v>2.5220060000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0299999999999999E-4</c:v>
+                  <c:v>3.4029050000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.5599999999999998E-4</c:v>
+                  <c:v>5.1445819999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -330,34 +324,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.7580000000000001E-3</c:v>
+                  <c:v>0.95196599999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8170000000000001E-3</c:v>
+                  <c:v>0.66829099999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8710000000000004E-3</c:v>
+                  <c:v>0.531752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7299999999999998E-3</c:v>
+                  <c:v>0.57339799999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7330000000000002E-3</c:v>
+                  <c:v>0.77741000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.2150000000000001E-3</c:v>
+                  <c:v>0.63341599999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.98E-3</c:v>
+                  <c:v>0.65261199999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5860000000000002E-3</c:v>
+                  <c:v>0.56630800000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5980000000000001E-3</c:v>
+                  <c:v>0.64118399999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.2950000000000002E-3</c:v>
+                  <c:v>0.71576399999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,34 +395,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.5639999999999999E-3</c:v>
+                  <c:v>8.9911549999999991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4359999999999999E-3</c:v>
+                  <c:v>10.204575999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9240000000000004E-3</c:v>
+                  <c:v>10.862017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.13E-3</c:v>
+                  <c:v>9.9232060000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4350000000000001E-3</c:v>
+                  <c:v>10.849819999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6880000000000003E-3</c:v>
+                  <c:v>10.052460999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8609999999999998E-3</c:v>
+                  <c:v>11.308913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9969999999999997E-3</c:v>
+                  <c:v>11.257792999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.9039999999999999E-3</c:v>
+                  <c:v>10.097391</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.2560000000000002E-3</c:v>
+                  <c:v>11.084801000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -759,13 +753,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.9389999999999993E-4</c:v>
+                  <c:v>3.9545254000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3582999999999998E-3</c:v>
+                  <c:v>0.67121010000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2195000000000002E-3</c:v>
+                  <c:v>10.4632133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -947,430 +941,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="105"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="5"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Comparison of Execution Time across Different No. Of Threads for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Dynamic and Static</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Parallel (Static)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:tint val="77000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$34:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$34:$C$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.036E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.2744999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.3369999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.5040000000000003E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2592-4AF7-A80E-A47BBD81D9F6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Parallel (Dynamic)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:shade val="76000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$34:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$34:$D$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.44E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.7099999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5775E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.1844999999999999E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2592-4AF7-A80E-A47BBD81D9F6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="529105152"/>
-        <c:axId val="538183616"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="529105152"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-PK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="538183616"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="538183616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-PK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="529105152"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-PK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-PK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
@@ -1417,12 +987,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
-  <a:schemeClr val="accent3"/>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2399,522 +1963,6 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3016,42 +2064,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2847975</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF66FC10-9A04-8D92-8AB5-95B4EB93CB25}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3379,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04018086-815F-4719-98C9-A9F79773E568}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3415,13 +2427,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>2.7099999999999997E-4</v>
+        <v>2.0874109999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>3.7580000000000001E-3</v>
+        <v>0.95196599999999998</v>
       </c>
       <c r="D3">
-        <v>3.5639999999999999E-3</v>
+        <v>8.9911549999999991</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3429,13 +2441,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>3.2299999999999999E-4</v>
+        <v>2.582166</v>
       </c>
       <c r="C4" s="2">
-        <v>3.8170000000000001E-3</v>
+        <v>0.66829099999999997</v>
       </c>
       <c r="D4">
-        <v>5.4359999999999999E-3</v>
+        <v>10.204575999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3443,13 +2455,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>2.14E-4</v>
+        <v>5.6043609999999999</v>
       </c>
       <c r="C5" s="2">
-        <v>5.8710000000000004E-3</v>
+        <v>0.531752</v>
       </c>
       <c r="D5">
-        <v>3.9240000000000004E-3</v>
+        <v>10.862017</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3457,13 +2469,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>1.8100000000000001E-4</v>
+        <v>7.0913029999999999</v>
       </c>
       <c r="C6" s="2">
-        <v>3.7299999999999998E-3</v>
+        <v>0.57339799999999996</v>
       </c>
       <c r="D6">
-        <v>4.13E-3</v>
+        <v>9.9232060000000004</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3471,13 +2483,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>2.05E-4</v>
+        <v>4.9783179999999998</v>
       </c>
       <c r="C7" s="2">
-        <v>2.7330000000000002E-3</v>
+        <v>0.77741000000000005</v>
       </c>
       <c r="D7">
-        <v>3.4350000000000001E-3</v>
+        <v>10.849819999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3485,13 +2497,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>6.8199999999999999E-4</v>
+        <v>1.6207819999999999</v>
       </c>
       <c r="C8" s="2">
-        <v>8.2150000000000001E-3</v>
+        <v>0.63341599999999998</v>
       </c>
       <c r="D8">
-        <v>4.6880000000000003E-3</v>
+        <v>10.052460999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3499,13 +2511,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>2.4399999999999999E-4</v>
+        <v>4.5114200000000002</v>
       </c>
       <c r="C9" s="2">
-        <v>3.98E-3</v>
+        <v>0.65261199999999997</v>
       </c>
       <c r="D9">
-        <v>3.8609999999999998E-3</v>
+        <v>11.308913</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3513,13 +2525,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1.6000000000000001E-4</v>
+        <v>2.5220060000000002</v>
       </c>
       <c r="C10" s="2">
-        <v>3.5860000000000002E-3</v>
+        <v>0.56630800000000003</v>
       </c>
       <c r="D10">
-        <v>4.9969999999999997E-3</v>
+        <v>11.257792999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3527,13 +2539,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>3.0299999999999999E-4</v>
+        <v>3.4029050000000001</v>
       </c>
       <c r="C11" s="2">
-        <v>3.5980000000000001E-3</v>
+        <v>0.64118399999999998</v>
       </c>
       <c r="D11">
-        <v>3.9039999999999999E-3</v>
+        <v>10.097391</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3541,90 +2553,50 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>3.5599999999999998E-4</v>
+        <v>5.1445819999999998</v>
       </c>
       <c r="C12" s="2">
-        <v>4.2950000000000002E-3</v>
+        <v>0.71576399999999996</v>
       </c>
       <c r="D12">
-        <v>4.2560000000000002E-3</v>
+        <v>11.084801000000001</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <f>AVERAGE(B3:B12)</f>
-        <v>2.9389999999999993E-4</v>
+        <v>3.9545254000000001</v>
       </c>
       <c r="C13" s="1">
         <f>AVERAGE(C3:C12)</f>
-        <v>4.3582999999999998E-3</v>
+        <v>0.67121010000000003</v>
       </c>
       <c r="D13" s="1">
         <f>AVERAGE(D3:D12)</f>
-        <v>4.2195000000000002E-3</v>
+        <v>10.4632133</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>1.036E-3</v>
-      </c>
-      <c r="D34">
-        <v>5.44E-4</v>
-      </c>
+      <c r="B34" s="2"/>
     </row>
     <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>6.2744999999999997E-3</v>
-      </c>
-      <c r="D35">
-        <v>7.7099999999999998E-3</v>
-      </c>
+      <c r="B35" s="2"/>
     </row>
     <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
-        <v>8</v>
-      </c>
-      <c r="C36">
-        <v>4.3369999999999997E-3</v>
-      </c>
-      <c r="D36">
-        <v>3.5775E-3</v>
-      </c>
+      <c r="B36" s="2"/>
     </row>
     <row r="37" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
-        <v>16</v>
-      </c>
-      <c r="C37">
-        <v>7.5040000000000003E-3</v>
-      </c>
-      <c r="D37">
-        <v>5.1844999999999999E-3</v>
-      </c>
+      <c r="B37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>